<commit_message>
biom homework 3 and lab 3
</commit_message>
<xml_diff>
--- a/LaTech/BIOM_510_Bioinstrumentation/HW/HW1.xlsx
+++ b/LaTech/BIOM_510_Bioinstrumentation/HW/HW1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunzi\Downloads\Study\LaTech\BIOM_510_Bioinstrumentation\HW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunzi\Documents\Study\LaTech\BIOM_510_Bioinstrumentation\HW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B96882B8-E558-4006-88AD-2C09DCE6701C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8277BDF-BEC4-4059-B1EE-D13B526B0255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="17460" windowHeight="20985" xr2:uid="{C2151E38-9E59-4B2A-8881-C4899E03746F}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{C2151E38-9E59-4B2A-8881-C4899E03746F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Magnitude</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Phase Shift</t>
+  </si>
+  <si>
+    <t>Phase Shift atan2</t>
   </si>
 </sst>
 </file>
@@ -459,11 +462,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Phase Shift</c:v>
+                  <c:v>Phase Shift atan2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -521,7 +524,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$7</c:f>
+              <c:f>Sheet1!$E$2:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -532,16 +535,16 @@
                   <c:v>12.667059925007866</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>162.3169243496925</c:v>
+                  <c:v>-17.683075650307487</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>94.049530896258688</c:v>
+                  <c:v>-85.950469103741327</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>90.401109170582984</c:v>
+                  <c:v>-89.598890829417016</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90.040107084372025</c:v>
+                  <c:v>-89.959892915627961</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1857,16 +1860,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>402078</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133564</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>92361</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>25410</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1893,23 +1896,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>233362</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>406164</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>69040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>538162</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>101364</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>139094</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDB6DC83-05DE-2417-32F6-C9520F8AD82F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1E76B2F-17A7-5408-1132-554D72B71573}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2227,15 +2230,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A039E79-0170-4B68-AFCE-BE92183E00A8}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2248,8 +2251,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -2265,8 +2271,12 @@
         <f>DEGREES(ATAN(A2/3)) - DEGREES(ATAN((10*A2)/(100 - A2^2)))</f>
         <v>1.3361564395333771</v>
       </c>
+      <c r="E2">
+        <f>DEGREES(ATAN2(3,A2))-DEGREES(ATAN2(100-A2^2,10*A2))</f>
+        <v>1.3361564395333771</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2279,11 +2289,15 @@
         <v>-29.956790605116218</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D7" si="2">DEGREES(ATAN(A3/3)) - DEGREES(ATAN((10*A3)/(100 - A3^2)))</f>
+        <f t="shared" ref="D3:D4" si="2">DEGREES(ATAN(A3/3)) - DEGREES(ATAN((10*A3)/(100 - A3^2)))</f>
         <v>12.667059925007866</v>
       </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E7" si="3">DEGREES(ATAN2(3,A3))-DEGREES(ATAN2(100-A3^2,10*A3))</f>
+        <v>12.667059925007866</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10.1</v>
       </c>
@@ -2299,8 +2313,12 @@
         <f t="shared" si="2"/>
         <v>162.3169243496925</v>
       </c>
+      <c r="E4">
+        <f t="shared" si="3"/>
+        <v>-17.683075650307487</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>100</v>
       </c>
@@ -2316,8 +2334,12 @@
         <f>DEGREES(ATAN(A5/3)) - DEGREES(ATAN((10*A5)/(100 - A5^2)))</f>
         <v>94.049530896258688</v>
       </c>
+      <c r="E5">
+        <f t="shared" si="3"/>
+        <v>-85.950469103741327</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1000</v>
       </c>
@@ -2333,8 +2355,12 @@
         <f>DEGREES(ATAN(A6/3)) - DEGREES(ATAN((10*A6)/(100 - A6^2)))</f>
         <v>90.401109170582984</v>
       </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>-89.598890829417016</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10000</v>
       </c>
@@ -2349,6 +2375,10 @@
       <c r="D7">
         <f>DEGREES(ATAN(A7/3)) - DEGREES(ATAN((10*A7)/(100 - A7^2)))</f>
         <v>90.040107084372025</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>-89.959892915627961</v>
       </c>
     </row>
   </sheetData>

</xml_diff>